<commit_message>
remodel offroad patterns for better readability
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -62,6 +62,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,7 +213,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,11 +221,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,10 +321,10 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.39"/>
@@ -328,8 +333,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="6.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="6.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="10" style="0" width="6.54"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,37 +379,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="E2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="I2" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="n">
+      <c r="L2" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="5" t="n">
         <v>3</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="K2" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>6</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -419,104 +423,115 @@
       </c>
       <c r="C3" s="10" t="n">
         <f aca="false">B3/B2*C2</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="10" t="n">
         <f aca="false">D$2/$C$2*$C3</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E3" s="10" t="n">
         <f aca="false">E$2/$C$2*$C3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="10" t="n">
         <f aca="false">F$2/$C$2*$C3</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G3" s="10" t="n">
         <f aca="false">G$2/$C$2*$C3</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3" s="10" t="n">
         <f aca="false">H$2/$C$2*$C3</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I3" s="10" t="n">
         <f aca="false">I$2/$C$2*$C3</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J3" s="10" t="n">
         <f aca="false">J$2/$C$2*$C3</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K3" s="10" t="n">
         <f aca="false">K$2/$C$2*$C3</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L3" s="10" t="n">
         <f aca="false">L$2/$C$2*$C3</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M3" s="10" t="n">
         <f aca="false">M$2/$C$2*$C3</f>
-        <v>12</v>
-      </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="N3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="11" t="n">
+        <f aca="false">C3-N3</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="13" t="n">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="13" t="n">
         <f aca="false">B4/B3*C3</f>
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <f aca="false">D$2/$C$2*$C4</f>
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="n">
-        <f aca="false">D$2/$C$2*$C4</f>
+      <c r="E4" s="13" t="n">
+        <f aca="false">E$2/$C$2*$C4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="13" t="n">
+        <f aca="false">F$2/$C$2*$C4</f>
+        <v>24</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <f aca="false">G$2/$C$2*$C4</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="13" t="n">
+        <f aca="false">H$2/$C$2*$C4</f>
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">E$2/$C$2*$C4</f>
+      <c r="I4" s="13" t="n">
+        <f aca="false">I$2/$C$2*$C4</f>
+        <v>9</v>
+      </c>
+      <c r="J4" s="13" t="n">
+        <f aca="false">J$2/$C$2*$C4</f>
+        <v>9</v>
+      </c>
+      <c r="K4" s="13" t="n">
+        <f aca="false">K$2/$C$2*$C4</f>
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">F$2/$C$2*$C4</f>
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <f aca="false">G$2/$C$2*$C4</f>
+      <c r="L4" s="13" t="n">
+        <f aca="false">L$2/$C$2*$C4</f>
+        <v>6</v>
+      </c>
+      <c r="M4" s="13" t="n">
+        <f aca="false">M$2/$C$2*$C4</f>
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="n">
-        <f aca="false">H$2/$C$2*$C4</f>
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <f aca="false">I$2/$C$2*$C4</f>
-        <v>12</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <f aca="false">J$2/$C$2*$C4</f>
-        <v>12</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <f aca="false">K$2/$C$2*$C4</f>
-        <v>15</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <f aca="false">L$2/$C$2*$C4</f>
-        <v>9</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <f aca="false">M$2/$C$2*$C4</f>
-        <v>18</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="N4" s="14" t="n">
+        <f aca="false">N$3/$C$3*$C4</f>
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="14" t="n">
+        <f aca="false">O$3/$C$3*$C4</f>
+        <v>28.5</v>
+      </c>
     </row>
     <row r="5" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
@@ -527,114 +542,115 @@
       </c>
       <c r="C5" s="10" t="n">
         <f aca="false">B5/B4*C4</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="10" t="n">
         <f aca="false">D$2/$C$2*$C5</f>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E5" s="10" t="n">
         <f aca="false">E$2/$C$2*$C5</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" s="10" t="n">
         <f aca="false">F$2/$C$2*$C5</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G5" s="10" t="n">
         <f aca="false">G$2/$C$2*$C5</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H5" s="10" t="n">
         <f aca="false">H$2/$C$2*$C5</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I5" s="10" t="n">
         <f aca="false">I$2/$C$2*$C5</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J5" s="10" t="n">
         <f aca="false">J$2/$C$2*$C5</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K5" s="10" t="n">
         <f aca="false">K$2/$C$2*$C5</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L5" s="10" t="n">
         <f aca="false">L$2/$C$2*$C5</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M5" s="10" t="n">
         <f aca="false">M$2/$C$2*$C5</f>
-        <v>24</v>
-      </c>
-      <c r="N5" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" s="10" t="n">
-        <f aca="false">C5-N5</f>
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="N5" s="15" t="n">
+        <f aca="false">N$3/$C$3*$C5</f>
+        <v>2</v>
+      </c>
+      <c r="O5" s="15" t="n">
+        <f aca="false">O$3/$C$3*$C5</f>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="14" t="n">
         <f aca="false">B6/B5*C5</f>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D6" s="14" t="n">
         <f aca="false">D$2/$C$2*$C6</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E6" s="14" t="n">
         <f aca="false">E$2/$C$2*$C6</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="14" t="n">
         <f aca="false">F$2/$C$2*$C6</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G6" s="14" t="n">
         <f aca="false">G$2/$C$2*$C6</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H6" s="14" t="n">
         <f aca="false">H$2/$C$2*$C6</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I6" s="14" t="n">
         <f aca="false">I$2/$C$2*$C6</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J6" s="14" t="n">
         <f aca="false">J$2/$C$2*$C6</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K6" s="14" t="n">
         <f aca="false">K$2/$C$2*$C6</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L6" s="14" t="n">
         <f aca="false">L$2/$C$2*$C6</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M6" s="14" t="n">
         <f aca="false">M$2/$C$2*$C6</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="N6" s="14" t="n">
-        <f aca="false">N$5/$C$5*$C6</f>
-        <v>5</v>
+        <f aca="false">N$3/$C$3*$C6</f>
+        <v>2.5</v>
       </c>
       <c r="O6" s="14" t="n">
-        <f aca="false">O$5/$C$5*$C6</f>
-        <v>40</v>
+        <f aca="false">O$3/$C$3*$C6</f>
+        <v>47.5</v>
       </c>
     </row>
     <row r="7" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,115 +662,115 @@
       </c>
       <c r="C7" s="10" t="n">
         <f aca="false">B7/B6*C6</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10" t="n">
         <f aca="false">D$2/$C$2*$C7</f>
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E7" s="10" t="n">
         <f aca="false">E$2/$C$2*$C7</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F7" s="10" t="n">
         <f aca="false">F$2/$C$2*$C7</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G7" s="10" t="n">
         <f aca="false">G$2/$C$2*$C7</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H7" s="10" t="n">
         <f aca="false">H$2/$C$2*$C7</f>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I7" s="10" t="n">
         <f aca="false">I$2/$C$2*$C7</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J7" s="10" t="n">
         <f aca="false">J$2/$C$2*$C7</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="K7" s="10" t="n">
         <f aca="false">K$2/$C$2*$C7</f>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="L7" s="10" t="n">
         <f aca="false">L$2/$C$2*$C7</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="M7" s="10" t="n">
         <f aca="false">M$2/$C$2*$C7</f>
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="N7" s="10" t="n">
         <f aca="false">N$5/$C$5*$C7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O7" s="10" t="n">
         <f aca="false">O$5/$C$5*$C7</f>
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="B8" s="13" t="n">
+      <c r="B8" s="7" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">B8/B7*C7</f>
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D8" s="14" t="n">
         <f aca="false">D$2/$C$2*$C8</f>
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E8" s="14" t="n">
         <f aca="false">E$2/$C$2*$C8</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F8" s="14" t="n">
         <f aca="false">F$2/$C$2*$C8</f>
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G8" s="14" t="n">
         <f aca="false">G$2/$C$2*$C8</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H8" s="14" t="n">
         <f aca="false">H$2/$C$2*$C8</f>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I8" s="14" t="n">
         <f aca="false">I$2/$C$2*$C8</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="J8" s="14" t="n">
         <f aca="false">J$2/$C$2*$C8</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K8" s="14" t="n">
         <f aca="false">K$2/$C$2*$C8</f>
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="L8" s="14" t="n">
         <f aca="false">L$2/$C$2*$C8</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M8" s="14" t="n">
         <f aca="false">M$2/$C$2*$C8</f>
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="N8" s="14" t="n">
         <f aca="false">N$5/$C$5*$C8</f>
-        <v>7</v>
+        <v>3.5</v>
       </c>
       <c r="O8" s="14" t="n">
         <f aca="false">O$5/$C$5*$C8</f>
-        <v>56</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="9" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,175 +782,175 @@
       </c>
       <c r="C9" s="10" t="n">
         <f aca="false">B9/B8*C8</f>
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D9" s="10" t="n">
         <f aca="false">D$2/$C$2*$C9</f>
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E9" s="10" t="n">
         <f aca="false">E$2/$C$2*$C9</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F9" s="10" t="n">
         <f aca="false">F$2/$C$2*$C9</f>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="G9" s="10" t="n">
         <f aca="false">G$2/$C$2*$C9</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H9" s="10" t="n">
         <f aca="false">H$2/$C$2*$C9</f>
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I9" s="10" t="n">
         <f aca="false">I$2/$C$2*$C9</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J9" s="10" t="n">
         <f aca="false">J$2/$C$2*$C9</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K9" s="10" t="n">
         <f aca="false">K$2/$C$2*$C9</f>
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L9" s="10" t="n">
         <f aca="false">L$2/$C$2*$C9</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="M9" s="10" t="n">
         <f aca="false">M$2/$C$2*$C9</f>
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="N9" s="10" t="n">
         <f aca="false">N$5/$C$5*$C9</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O9" s="10" t="n">
         <f aca="false">O$5/$C$5*$C9</f>
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="B10" s="13" t="n">
+      <c r="B10" s="7" t="n">
         <v>9</v>
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">B10/B9*C9</f>
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D10" s="14" t="n">
         <f aca="false">D$2/$C$2*$C10</f>
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E10" s="14" t="n">
         <f aca="false">E$2/$C$2*$C10</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F10" s="14" t="n">
         <f aca="false">F$2/$C$2*$C10</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G10" s="14" t="n">
         <f aca="false">G$2/$C$2*$C10</f>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H10" s="14" t="n">
         <f aca="false">H$2/$C$2*$C10</f>
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="I10" s="14" t="n">
         <f aca="false">I$2/$C$2*$C10</f>
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J10" s="14" t="n">
         <f aca="false">J$2/$C$2*$C10</f>
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="K10" s="14" t="n">
         <f aca="false">K$2/$C$2*$C10</f>
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="L10" s="14" t="n">
         <f aca="false">L$2/$C$2*$C10</f>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="M10" s="14" t="n">
         <f aca="false">M$2/$C$2*$C10</f>
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N10" s="14" t="n">
         <f aca="false">N$5/$C$5*$C10</f>
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="O10" s="14" t="n">
         <f aca="false">O$5/$C$5*$C10</f>
-        <v>72</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="11" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
+      <c r="A11" s="16" t="n">
         <v>21</v>
       </c>
-      <c r="B11" s="15" t="n">
+      <c r="B11" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="16" t="n">
+      <c r="C11" s="17" t="n">
         <f aca="false">B11/B10*C10</f>
+        <v>100</v>
+      </c>
+      <c r="D11" s="17" t="n">
+        <f aca="false">D$2/$C$2*$C11</f>
         <v>90</v>
       </c>
-      <c r="D11" s="16" t="n">
-        <f aca="false">D$2/$C$2*$C11</f>
+      <c r="E11" s="17" t="n">
+        <f aca="false">E$2/$C$2*$C11</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="17" t="n">
+        <f aca="false">F$2/$C$2*$C11</f>
+        <v>80</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <f aca="false">G$2/$C$2*$C11</f>
+        <v>20</v>
+      </c>
+      <c r="H11" s="17" t="n">
+        <f aca="false">H$2/$C$2*$C11</f>
         <v>70</v>
       </c>
-      <c r="E11" s="16" t="n">
-        <f aca="false">E$2/$C$2*$C11</f>
+      <c r="I11" s="17" t="n">
+        <f aca="false">I$2/$C$2*$C11</f>
+        <v>30</v>
+      </c>
+      <c r="J11" s="17" t="n">
+        <f aca="false">J$2/$C$2*$C11</f>
+        <v>30</v>
+      </c>
+      <c r="K11" s="17" t="n">
+        <f aca="false">K$2/$C$2*$C11</f>
         <v>20</v>
       </c>
-      <c r="F11" s="16" t="n">
-        <f aca="false">F$2/$C$2*$C11</f>
-        <v>60</v>
-      </c>
-      <c r="G11" s="16" t="n">
-        <f aca="false">G$2/$C$2*$C11</f>
+      <c r="L11" s="17" t="n">
+        <f aca="false">L$2/$C$2*$C11</f>
+        <v>20</v>
+      </c>
+      <c r="M11" s="17" t="n">
+        <f aca="false">M$2/$C$2*$C11</f>
         <v>30</v>
-      </c>
-      <c r="H11" s="16" t="n">
-        <f aca="false">H$2/$C$2*$C11</f>
-        <v>50</v>
-      </c>
-      <c r="I11" s="16" t="n">
-        <f aca="false">I$2/$C$2*$C11</f>
-        <v>40</v>
-      </c>
-      <c r="J11" s="16" t="n">
-        <f aca="false">J$2/$C$2*$C11</f>
-        <v>40</v>
-      </c>
-      <c r="K11" s="16" t="n">
-        <f aca="false">K$2/$C$2*$C11</f>
-        <v>50</v>
-      </c>
-      <c r="L11" s="16" t="n">
-        <f aca="false">L$2/$C$2*$C11</f>
-        <v>30</v>
-      </c>
-      <c r="M11" s="16" t="n">
-        <f aca="false">M$2/$C$2*$C11</f>
-        <v>60</v>
       </c>
       <c r="N11" s="10" t="n">
         <f aca="false">N$5/$C$5*$C11</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O11" s="10" t="n">
         <f aca="false">O$5/$C$5*$C11</f>
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>